<commit_message>
measurement global points satisfied
</commit_message>
<xml_diff>
--- a/data/trivial.xlsx
+++ b/data/trivial.xlsx
@@ -164,7 +164,7 @@
   <dimension ref="A1:N102"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2:J102"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="1" sqref="J2:J102 D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5380,10 +5380,10 @@
         <v>0</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L2" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -5430,10 +5430,10 @@
         <v>0</v>
       </c>
       <c r="J3" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L3" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -5480,10 +5480,10 @@
         <v>0</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L4" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -5530,10 +5530,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L5" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -5580,10 +5580,10 @@
         <v>0</v>
       </c>
       <c r="J6" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K6" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L6" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -5630,10 +5630,10 @@
         <v>0</v>
       </c>
       <c r="J7" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L7" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -5680,10 +5680,10 @@
         <v>0</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K8" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L8" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -5730,10 +5730,10 @@
         <v>0</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K9" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L9" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -5780,10 +5780,10 @@
         <v>0</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K10" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L10" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -5830,10 +5830,10 @@
         <v>0</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K11" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L11" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -5880,10 +5880,10 @@
         <v>0</v>
       </c>
       <c r="J12" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K12" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L12" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -5930,10 +5930,10 @@
         <v>0</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K13" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L13" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -5980,10 +5980,10 @@
         <v>0</v>
       </c>
       <c r="J14" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K14" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L14" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -6030,10 +6030,10 @@
         <v>0</v>
       </c>
       <c r="J15" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K15" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L15" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -6080,10 +6080,10 @@
         <v>0</v>
       </c>
       <c r="J16" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K16" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L16" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -6130,10 +6130,10 @@
         <v>0</v>
       </c>
       <c r="J17" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K17" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L17" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -6180,10 +6180,10 @@
         <v>0</v>
       </c>
       <c r="J18" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K18" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L18" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -6230,10 +6230,10 @@
         <v>0</v>
       </c>
       <c r="J19" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K19" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L19" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -6280,10 +6280,10 @@
         <v>0</v>
       </c>
       <c r="J20" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K20" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L20" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -6330,10 +6330,10 @@
         <v>0</v>
       </c>
       <c r="J21" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K21" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L21" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -6380,10 +6380,10 @@
         <v>0</v>
       </c>
       <c r="J22" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K22" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L22" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -6430,10 +6430,10 @@
         <v>0</v>
       </c>
       <c r="J23" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K23" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L23" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -6480,10 +6480,10 @@
         <v>0</v>
       </c>
       <c r="J24" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K24" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L24" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -6530,10 +6530,10 @@
         <v>0</v>
       </c>
       <c r="J25" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K25" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L25" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -6580,10 +6580,10 @@
         <v>0</v>
       </c>
       <c r="J26" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K26" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L26" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -6630,10 +6630,10 @@
         <v>0</v>
       </c>
       <c r="J27" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K27" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L27" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -6680,10 +6680,10 @@
         <v>0</v>
       </c>
       <c r="J28" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K28" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L28" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -6730,10 +6730,10 @@
         <v>0</v>
       </c>
       <c r="J29" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K29" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L29" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -6780,10 +6780,10 @@
         <v>0</v>
       </c>
       <c r="J30" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K30" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L30" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -6830,10 +6830,10 @@
         <v>0</v>
       </c>
       <c r="J31" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K31" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L31" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -6880,10 +6880,10 @@
         <v>0</v>
       </c>
       <c r="J32" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K32" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L32" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -6930,10 +6930,10 @@
         <v>0</v>
       </c>
       <c r="J33" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K33" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L33" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -6980,10 +6980,10 @@
         <v>0</v>
       </c>
       <c r="J34" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K34" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L34" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -7030,10 +7030,10 @@
         <v>0</v>
       </c>
       <c r="J35" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K35" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L35" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -7080,10 +7080,10 @@
         <v>0</v>
       </c>
       <c r="J36" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K36" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L36" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -7130,10 +7130,10 @@
         <v>0</v>
       </c>
       <c r="J37" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K37" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L37" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -7180,10 +7180,10 @@
         <v>0</v>
       </c>
       <c r="J38" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K38" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L38" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -7230,10 +7230,10 @@
         <v>0</v>
       </c>
       <c r="J39" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K39" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L39" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -7280,10 +7280,10 @@
         <v>0</v>
       </c>
       <c r="J40" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K40" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L40" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -7330,10 +7330,10 @@
         <v>0</v>
       </c>
       <c r="J41" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K41" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L41" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -7380,10 +7380,10 @@
         <v>0</v>
       </c>
       <c r="J42" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K42" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L42" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -7430,10 +7430,10 @@
         <v>0</v>
       </c>
       <c r="J43" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K43" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L43" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -7480,10 +7480,10 @@
         <v>0</v>
       </c>
       <c r="J44" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K44" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L44" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -7530,10 +7530,10 @@
         <v>0</v>
       </c>
       <c r="J45" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K45" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L45" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -7580,10 +7580,10 @@
         <v>0</v>
       </c>
       <c r="J46" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K46" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L46" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -7630,10 +7630,10 @@
         <v>0</v>
       </c>
       <c r="J47" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K47" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L47" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -7680,10 +7680,10 @@
         <v>0</v>
       </c>
       <c r="J48" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K48" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L48" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -7730,10 +7730,10 @@
         <v>0</v>
       </c>
       <c r="J49" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K49" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L49" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -7780,10 +7780,10 @@
         <v>0</v>
       </c>
       <c r="J50" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K50" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L50" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -7830,10 +7830,10 @@
         <v>0</v>
       </c>
       <c r="J51" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K51" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L51" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -7880,10 +7880,10 @@
         <v>0</v>
       </c>
       <c r="J52" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K52" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L52" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -7930,10 +7930,10 @@
         <v>0</v>
       </c>
       <c r="J53" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K53" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L53" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -7980,10 +7980,10 @@
         <v>0</v>
       </c>
       <c r="J54" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K54" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L54" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -8030,10 +8030,10 @@
         <v>0</v>
       </c>
       <c r="J55" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K55" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L55" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -8080,10 +8080,10 @@
         <v>0</v>
       </c>
       <c r="J56" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K56" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L56" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -8130,10 +8130,10 @@
         <v>0</v>
       </c>
       <c r="J57" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K57" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L57" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -8180,10 +8180,10 @@
         <v>0</v>
       </c>
       <c r="J58" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K58" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L58" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -8230,10 +8230,10 @@
         <v>0</v>
       </c>
       <c r="J59" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K59" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L59" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -8280,10 +8280,10 @@
         <v>0</v>
       </c>
       <c r="J60" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K60" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L60" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -8330,10 +8330,10 @@
         <v>0</v>
       </c>
       <c r="J61" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K61" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L61" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -8380,10 +8380,10 @@
         <v>0</v>
       </c>
       <c r="J62" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K62" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L62" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -8430,10 +8430,10 @@
         <v>0</v>
       </c>
       <c r="J63" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K63" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L63" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -8480,10 +8480,10 @@
         <v>0</v>
       </c>
       <c r="J64" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K64" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L64" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -8530,10 +8530,10 @@
         <v>0</v>
       </c>
       <c r="J65" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K65" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L65" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -8580,10 +8580,10 @@
         <v>0</v>
       </c>
       <c r="J66" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K66" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L66" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -8630,10 +8630,10 @@
         <v>0</v>
       </c>
       <c r="J67" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K67" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L67" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -8680,10 +8680,10 @@
         <v>0</v>
       </c>
       <c r="J68" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K68" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L68" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -8730,10 +8730,10 @@
         <v>0</v>
       </c>
       <c r="J69" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K69" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L69" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -8780,10 +8780,10 @@
         <v>0</v>
       </c>
       <c r="J70" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K70" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L70" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -8830,10 +8830,10 @@
         <v>0</v>
       </c>
       <c r="J71" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K71" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L71" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -8880,10 +8880,10 @@
         <v>0</v>
       </c>
       <c r="J72" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K72" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L72" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -8930,10 +8930,10 @@
         <v>0</v>
       </c>
       <c r="J73" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K73" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L73" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -8980,10 +8980,10 @@
         <v>0</v>
       </c>
       <c r="J74" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K74" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L74" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -9030,10 +9030,10 @@
         <v>0</v>
       </c>
       <c r="J75" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K75" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L75" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -9080,10 +9080,10 @@
         <v>0</v>
       </c>
       <c r="J76" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K76" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L76" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -9130,10 +9130,10 @@
         <v>0</v>
       </c>
       <c r="J77" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K77" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L77" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -9180,10 +9180,10 @@
         <v>0</v>
       </c>
       <c r="J78" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K78" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L78" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -9230,10 +9230,10 @@
         <v>0</v>
       </c>
       <c r="J79" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K79" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L79" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -9280,10 +9280,10 @@
         <v>0</v>
       </c>
       <c r="J80" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K80" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L80" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -9330,10 +9330,10 @@
         <v>0</v>
       </c>
       <c r="J81" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K81" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L81" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -9380,10 +9380,10 @@
         <v>0</v>
       </c>
       <c r="J82" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K82" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L82" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -9430,10 +9430,10 @@
         <v>0</v>
       </c>
       <c r="J83" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K83" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L83" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -9480,10 +9480,10 @@
         <v>0</v>
       </c>
       <c r="J84" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K84" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L84" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -9530,10 +9530,10 @@
         <v>0</v>
       </c>
       <c r="J85" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K85" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L85" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -9580,10 +9580,10 @@
         <v>0</v>
       </c>
       <c r="J86" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K86" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L86" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -9630,10 +9630,10 @@
         <v>0</v>
       </c>
       <c r="J87" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K87" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L87" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -9680,10 +9680,10 @@
         <v>0</v>
       </c>
       <c r="J88" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K88" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L88" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -9730,10 +9730,10 @@
         <v>0</v>
       </c>
       <c r="J89" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K89" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L89" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -9780,10 +9780,10 @@
         <v>0</v>
       </c>
       <c r="J90" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K90" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L90" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -9830,10 +9830,10 @@
         <v>0</v>
       </c>
       <c r="J91" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K91" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L91" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -9880,10 +9880,10 @@
         <v>0</v>
       </c>
       <c r="J92" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K92" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L92" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -9930,10 +9930,10 @@
         <v>0</v>
       </c>
       <c r="J93" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K93" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L93" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -9980,10 +9980,10 @@
         <v>0</v>
       </c>
       <c r="J94" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K94" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L94" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -10030,10 +10030,10 @@
         <v>0</v>
       </c>
       <c r="J95" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K95" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L95" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -10080,10 +10080,10 @@
         <v>0</v>
       </c>
       <c r="J96" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K96" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L96" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -10130,10 +10130,10 @@
         <v>0</v>
       </c>
       <c r="J97" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K97" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L97" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -10180,10 +10180,10 @@
         <v>0</v>
       </c>
       <c r="J98" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K98" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L98" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -10230,10 +10230,10 @@
         <v>0</v>
       </c>
       <c r="J99" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K99" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L99" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -10280,10 +10280,10 @@
         <v>0</v>
       </c>
       <c r="J100" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K100" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L100" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -10330,10 +10330,10 @@
         <v>0</v>
       </c>
       <c r="J101" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K101" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L101" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>
@@ -10380,10 +10380,10 @@
         <v>0</v>
       </c>
       <c r="J102" s="0" t="n">
-        <v>0.001309</v>
+        <v>0.003927</v>
       </c>
       <c r="K102" s="0" t="n">
-        <v>1</v>
+        <v>0.99999</v>
       </c>
       <c r="L102" s="0" t="n">
         <f aca="false">RANDBETWEEN(-500,500)*0.001</f>

</xml_diff>

<commit_message>
make a longer trivial data and then test again. 1sec is too short
</commit_message>
<xml_diff>
--- a/data/trivial.xlsx
+++ b/data/trivial.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="IMU0" sheetId="1" state="visible" r:id="rId2"/>
@@ -163,8 +163,8 @@
   </sheetPr>
   <dimension ref="A1:N102"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="1" sqref="J2:J102 D17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5291,8 +5291,8 @@
   </sheetPr>
   <dimension ref="A1:N102"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2:J102"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G102" activeCellId="0" sqref="G102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -10417,7 +10417,7 @@
   <dimension ref="A1:N102"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="J2:J102 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -15542,7 +15542,7 @@
   <dimension ref="A1:N102"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="J2:J102 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>